<commit_message>
Fix incorrect date in sample file
</commit_message>
<xml_diff>
--- a/tests/fixtures/br-sample.xlsx
+++ b/tests/fixtures/br-sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lenon/dev/stonks/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACA5649-4076-AB4E-B825-BD56B669F53E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0177D772-411A-1149-B313-F11B661A2B7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14400" xr2:uid="{B3D269A4-9DC6-0A44-9507-02E24F504701}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14400" activeTab="2" xr2:uid="{B3D269A4-9DC6-0A44-9507-02E24F504701}"/>
   </bookViews>
   <sheets>
     <sheet name="confirmations" sheetId="1" r:id="rId1"/>
@@ -521,7 +521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E0AE5C6-7C9B-A440-B8A5-8D416F6122EA}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1106,7 +1106,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32D1046C-19B3-864E-B7C3-368B60E7F34C}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1223,9 +1225,7 @@
       <c r="J3" s="2">
         <v>10.5</v>
       </c>
-      <c r="K3" s="1">
-        <v>44602</v>
-      </c>
+      <c r="K3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Increase the gap between events dates
Allow new events to be added between those events.
</commit_message>
<xml_diff>
--- a/tests/fixtures/br-sample.xlsx
+++ b/tests/fixtures/br-sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lenon/dev/stonks/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0177D772-411A-1149-B313-F11B661A2B7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B89DD1B-C75D-CF4B-9E77-39E0880CA6C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14400" activeTab="2" xr2:uid="{B3D269A4-9DC6-0A44-9507-02E24F504701}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14400" xr2:uid="{B3D269A4-9DC6-0A44-9507-02E24F504701}"/>
   </bookViews>
   <sheets>
     <sheet name="confirmations" sheetId="1" r:id="rId1"/>
@@ -521,7 +521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E0AE5C6-7C9B-A440-B8A5-8D416F6122EA}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -588,7 +588,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>44563</v>
+        <v>44576</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -614,7 +614,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>44564</v>
+        <v>44592</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -640,7 +640,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>44565</v>
+        <v>44593</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -666,7 +666,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>44566</v>
+        <v>44607</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
@@ -692,7 +692,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>44567</v>
+        <v>44620</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -718,7 +718,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>44567</v>
+        <v>44620</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
@@ -744,7 +744,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>44568</v>
+        <v>44621</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
@@ -770,7 +770,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>44569</v>
+        <v>44635</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
@@ -804,7 +804,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A2" sqref="A2:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -859,7 +859,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>44563</v>
+        <v>44576</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -879,7 +879,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>44563</v>
+        <v>44576</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -899,7 +899,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>44564</v>
+        <v>44592</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -919,7 +919,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>44564</v>
+        <v>44592</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
@@ -939,7 +939,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>44565</v>
+        <v>44593</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
@@ -959,7 +959,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>44565</v>
+        <v>44593</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
@@ -979,7 +979,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>44566</v>
+        <v>44607</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
@@ -999,7 +999,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>44567</v>
+        <v>44620</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
@@ -1019,7 +1019,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>44567</v>
+        <v>44620</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
@@ -1039,7 +1039,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>44567</v>
+        <v>44620</v>
       </c>
       <c r="B12" t="s">
         <v>0</v>
@@ -1059,7 +1059,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>44568</v>
+        <v>44621</v>
       </c>
       <c r="B13" t="s">
         <v>0</v>
@@ -1079,7 +1079,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>44569</v>
+        <v>44635</v>
       </c>
       <c r="B14" t="s">
         <v>0</v>
@@ -1106,7 +1106,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32D1046C-19B3-864E-B7C3-368B60E7F34C}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1176,10 +1176,10 @@
         <v>44562</v>
       </c>
       <c r="F2" s="1">
-        <v>44563</v>
+        <v>44571</v>
       </c>
       <c r="G2" s="1">
-        <v>44564</v>
+        <v>44572</v>
       </c>
       <c r="H2">
         <v>100</v>
@@ -1191,12 +1191,12 @@
         <v>50.1</v>
       </c>
       <c r="K2" s="1">
-        <v>44571</v>
+        <v>44576</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>44593</v>
+        <v>44652</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -1208,13 +1208,13 @@
         <v>12</v>
       </c>
       <c r="E3" s="1">
-        <v>44593</v>
+        <v>44652</v>
       </c>
       <c r="F3" s="1">
-        <v>44594</v>
+        <v>44661</v>
       </c>
       <c r="G3" s="1">
-        <v>44595</v>
+        <v>44662</v>
       </c>
       <c r="H3">
         <v>50</v>
@@ -1237,7 +1237,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1260,7 +1260,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>44566</v>
+        <v>44607</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -1271,7 +1271,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>44571</v>
+        <v>44651</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -1289,7 +1289,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF899857-DF4E-4041-906C-06C3EF3331F4}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1315,7 +1317,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>44571</v>
+        <v>44651</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -1368,7 +1370,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>44621</v>
+        <v>44652</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>

</xml_diff>